<commit_message>
maj interface + maj nonlieu (communes)
</commit_message>
<xml_diff>
--- a/passeports/données/calcullegende.xlsx
+++ b/passeports/données/calcullegende.xlsx
@@ -16,28 +16,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>AF 1545.9379931518124</t>
-  </si>
-  <si>
-    <t>AO 2206.3918880281635</t>
-  </si>
-  <si>
-    <t>AL 62.70610953786672</t>
-  </si>
-  <si>
-    <t>AF875.1821178268001</t>
-  </si>
-  <si>
-    <t> 40 075 016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>perimètre de l'équateur</t>
+  </si>
+  <si>
+    <t>wikipedia</t>
+  </si>
+  <si>
+    <t>longueur total du demi-equateur</t>
+  </si>
+  <si>
+    <t>&lt;svg&gt;</t>
+  </si>
+  <si>
+    <t>&lt;path id="milieu" fill="none" stroke="#6C6C6C" stroke-width="6" d="M375,333.3h14h13.9h13.9h13.8"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;path id="cote" fill="none" stroke="#6C6C6C" stroke-width="6" d="M675.7,333.3h4.5h3.9h3.3h2.7h2.1h1.5h0.9l0.3,0"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;path id="total" fill="none" stroke="#6C6C6C" stroke-width="6" d="M55,333.3h0.3h0.9h1.5h2.1h2.7h3.3h3.9h4.5h5.1H85h6.2h6.7h7.2 h7.8h8.3h8.7h9.2h9.7h10.1h10.5h10.9h11.3h11.6H215h12.2h12.5h12.8h13h13.2h13.4h13.6h13.7h13.8h13.9H361h14h14h13.9h13.9h13.8h13.7 h13.6h13.4h13.2h13h12.8h12.5H535h11.9h11.6h11.3h10.9h10.5h10.1h9.7h9.2h8.7h8.3h7.8h7.2h6.7h6.2h5.6h5.1h4.5h3.9h3.3h2.7h2.1h1.5 h0.9l0.3,0"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>pour calcule getTotalLengt:</t>
+  </si>
+  <si>
+    <t>55.5999755859375</t>
+  </si>
+  <si>
+    <t>19.20001220703125</t>
+  </si>
+  <si>
+    <t>périmètre</t>
+  </si>
+  <si>
+    <t>milieu</t>
+  </si>
+  <si>
+    <t>milieu part</t>
+  </si>
+  <si>
+    <t>cote</t>
+  </si>
+  <si>
+    <t>cote part</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.0\ _€_-;\-* #,##0.0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.0\ _€_-;\-* #,##0.0\ _€_-;_-* &quot;-&quot;?\ _€_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,14 +114,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,35 +418,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="62.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1">
+        <v>40075016</v>
+      </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <f>B1/2</f>
+        <v>20037508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>10/B2</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <f>B3*B6</f>
+        <v>313086.0625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>20/B2</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <f>B3*B8</f>
+        <v>626172.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>